<commit_message>
I hope last push
</commit_message>
<xml_diff>
--- a/experiment_data/model_tournament/model_tournament_mich1.xlsx
+++ b/experiment_data/model_tournament/model_tournament_mich1.xlsx
@@ -1322,15 +1322,37 @@
           <t>claude-3-5-sonnet-latest</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="inlineStr"/>
-      <c r="K26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>RED</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>2.166666666666667</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>cards finished</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>6</v>
+      </c>
+      <c r="J26" t="n">
+        <v>5</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
       <c r="L26" t="inlineStr"/>
     </row>
     <row r="27">

</xml_diff>